<commit_message>
Begin armed conflict matrices
</commit_message>
<xml_diff>
--- a/tables/distance_regression.xlsx
+++ b/tables/distance_regression.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\message_trade\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7419BF6D-FFD9-41F9-8CEB-8C1B723EF170}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3657BA5D-EECA-43D0-AD32-B92303248878}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{633E85D1-71FF-4EC7-8367-D3D913311F50}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{633E85D1-71FF-4EC7-8367-D3D913311F50}"/>
   </bookViews>
   <sheets>
     <sheet name="All regions" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -333,15 +333,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -351,9 +354,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -672,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E223A6-EBA7-43CF-A8B2-9894ADF7E6FB}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -688,30 +688,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="20" t="s">
         <v>31</v>
       </c>
     </row>
@@ -719,61 +719,121 @@
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="5"/>
+      <c r="B3" s="17">
+        <v>-1.29683294902167E-3</v>
+      </c>
+      <c r="C3" s="18">
+        <v>7.5797004021796005E-5</v>
+      </c>
+      <c r="D3" s="18">
+        <v>-17.109290344098</v>
+      </c>
+      <c r="E3" s="18">
+        <v>1.4251243699256201E-65</v>
+      </c>
+      <c r="F3" s="5">
+        <v>18066.2709044121</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="8"/>
+      <c r="B4" s="13">
+        <v>-1.6242725856548401E-5</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1.16549497315425E-6</v>
+      </c>
+      <c r="D4" s="14">
+        <v>-13.9363328291239</v>
+      </c>
+      <c r="E4" s="14">
+        <v>7.4572802380457905E-44</v>
+      </c>
+      <c r="F4" s="8">
+        <v>94.824046993718795</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="3"/>
+      <c r="B5" s="11">
+        <v>-2.7414516893610702E-3</v>
+      </c>
+      <c r="C5" s="12">
+        <v>1.3168796473137499E-4</v>
+      </c>
+      <c r="D5" s="12">
+        <v>-20.8177846392663</v>
+      </c>
+      <c r="E5" s="12">
+        <v>2.7890858422070198E-95</v>
+      </c>
+      <c r="F5" s="3">
+        <v>17620.421472280101</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="8"/>
+      <c r="B6" s="13">
+        <v>-1.0235181544028801E-2</v>
+      </c>
+      <c r="C6" s="14">
+        <v>6.3336476014343201E-4</v>
+      </c>
+      <c r="D6" s="14">
+        <v>-16.160011083835801</v>
+      </c>
+      <c r="E6" s="14">
+        <v>3.6371163929086999E-58</v>
+      </c>
+      <c r="F6" s="8">
+        <v>108930.73846740799</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="3"/>
+      <c r="B7" s="11">
+        <v>-2.54357619273104E-3</v>
+      </c>
+      <c r="C7" s="12">
+        <v>1.78483131083352E-4</v>
+      </c>
+      <c r="D7" s="12">
+        <v>-14.2510733495771</v>
+      </c>
+      <c r="E7" s="12">
+        <v>6.9210688052363497E-46</v>
+      </c>
+      <c r="F7" s="3">
+        <v>17886.750467680999</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="10"/>
+      <c r="B8" s="15">
+        <v>-1.2815041704246999E-3</v>
+      </c>
+      <c r="C8" s="16">
+        <v>9.1988607959879299E-5</v>
+      </c>
+      <c r="D8" s="16">
+        <v>-13.931118198718901</v>
+      </c>
+      <c r="E8" s="16">
+        <v>4.6866764081426201E-44</v>
+      </c>
+      <c r="F8" s="10">
+        <v>7788.5179683664801</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -788,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17B115ED-F9C7-46C6-A7E7-3755AAE90618}">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A48" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="J87" sqref="J87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -804,30 +864,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="20" t="s">
         <v>31</v>
       </c>
     </row>
@@ -835,87 +895,147 @@
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="5"/>
+      <c r="B3" s="17">
+        <v>-1.75169100165782E-4</v>
+      </c>
+      <c r="C3" s="18">
+        <v>7.1064298564655999E-5</v>
+      </c>
+      <c r="D3" s="18">
+        <v>-2.4649381433971298</v>
+      </c>
+      <c r="E3" s="18">
+        <v>1.3712979650889599E-2</v>
+      </c>
+      <c r="F3" s="5">
+        <v>2294.92627975816</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="8"/>
+      <c r="B4" s="13">
+        <v>-2.01903479796675E-6</v>
+      </c>
+      <c r="C4" s="14">
+        <v>5.3963125282652899E-7</v>
+      </c>
+      <c r="D4" s="14">
+        <v>-3.7415082751254198</v>
+      </c>
+      <c r="E4" s="14">
+        <v>2.0117113811258001E-4</v>
+      </c>
+      <c r="F4" s="8">
+        <v>5.19787111684726</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="3"/>
+      <c r="B5" s="11">
+        <v>-9.5501471583259794E-5</v>
+      </c>
+      <c r="C5" s="12">
+        <v>4.5974776178237497E-5</v>
+      </c>
+      <c r="D5" s="12">
+        <v>-2.0772579993215099</v>
+      </c>
+      <c r="E5" s="12">
+        <v>3.7980742353824801E-2</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1521.3687044409801</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="8"/>
+      <c r="B6" s="13">
+        <v>1.2941993275445601E-3</v>
+      </c>
+      <c r="C6" s="14">
+        <v>7.5654132952535905E-4</v>
+      </c>
+      <c r="D6" s="14">
+        <v>1.7106789504236599</v>
+      </c>
+      <c r="E6" s="14">
+        <v>8.7637420464929602E-2</v>
+      </c>
+      <c r="F6" s="8">
+        <v>23252.6474708606</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="3"/>
+      <c r="B7" s="11">
+        <v>-6.9466181065648005E-5</v>
+      </c>
+      <c r="C7" s="12">
+        <v>5.2361431311582101E-5</v>
+      </c>
+      <c r="D7" s="12">
+        <v>-1.3266669631752901</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0.18475606298821401</v>
+      </c>
+      <c r="F7" s="3">
+        <v>712.27037696596597</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="10"/>
+      <c r="B8" s="15">
+        <v>-2.7073296264935198E-4</v>
+      </c>
+      <c r="C8" s="16">
+        <v>2.1176384951273202E-5</v>
+      </c>
+      <c r="D8" s="16">
+        <v>-12.784663825875301</v>
+      </c>
+      <c r="E8" s="16">
+        <v>4.0847322240736197E-37</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1557.36277458515</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="20" t="s">
         <v>31</v>
       </c>
     </row>
@@ -923,87 +1043,147 @@
       <c r="A12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="5"/>
+      <c r="B12" s="17">
+        <v>1.05199395140122E-2</v>
+      </c>
+      <c r="C12" s="18">
+        <v>1.99390126114496E-3</v>
+      </c>
+      <c r="D12" s="18">
+        <v>5.2760584082139399</v>
+      </c>
+      <c r="E12" s="18">
+        <v>1.37129051914092E-7</v>
+      </c>
+      <c r="F12" s="5">
+        <v>29596.100723325799</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="8"/>
+      <c r="B13" s="13">
+        <v>-5.9639023980692299E-5</v>
+      </c>
+      <c r="C13" s="14">
+        <v>9.0940097491341897E-5</v>
+      </c>
+      <c r="D13" s="14">
+        <v>-0.65580558659913801</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.51269917925292696</v>
+      </c>
+      <c r="F13" s="8">
+        <v>53.523411993214403</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="3"/>
+      <c r="B14" s="11">
+        <v>4.6812740534090701E-2</v>
+      </c>
+      <c r="C14" s="12">
+        <v>1.1841340798022799E-2</v>
+      </c>
+      <c r="D14" s="12">
+        <v>3.9533310739529899</v>
+      </c>
+      <c r="E14" s="12">
+        <v>8.6338878444891005E-5</v>
+      </c>
+      <c r="F14" s="3">
+        <v>47268.681651053797</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="8"/>
+      <c r="B15" s="13">
+        <v>3.2029726653223498E-3</v>
+      </c>
+      <c r="C15" s="14">
+        <v>1.7268090703511998E-2</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0.18548504987125899</v>
+      </c>
+      <c r="E15" s="14">
+        <v>0.85291129039656799</v>
+      </c>
+      <c r="F15" s="8">
+        <v>126158.331560231</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="3"/>
+      <c r="B16" s="11">
+        <v>7.7824752316982401E-3</v>
+      </c>
+      <c r="C16" s="12">
+        <v>1.35387604793771E-3</v>
+      </c>
+      <c r="D16" s="12">
+        <v>5.7482922779769101</v>
+      </c>
+      <c r="E16" s="12">
+        <v>1.32063082909205E-8</v>
+      </c>
+      <c r="F16" s="3">
+        <v>13990.2559047348</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="10"/>
+      <c r="B17" s="15">
+        <v>-5.2731176862390499E-3</v>
+      </c>
+      <c r="C17" s="16">
+        <v>9.3892505031783005E-4</v>
+      </c>
+      <c r="D17" s="16">
+        <v>-5.6161220583624596</v>
+      </c>
+      <c r="E17" s="16">
+        <v>2.2429200791757099E-8</v>
+      </c>
+      <c r="F17" s="10">
+        <v>12280.5386634444</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="23"/>
     </row>
     <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="20" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1011,87 +1191,147 @@
       <c r="A21" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="5"/>
+      <c r="B21" s="17">
+        <v>-3.5516888598578999E-4</v>
+      </c>
+      <c r="C21" s="18">
+        <v>4.8112692219530099E-5</v>
+      </c>
+      <c r="D21" s="18">
+        <v>-7.3820206187010804</v>
+      </c>
+      <c r="E21" s="18">
+        <v>1.6836929992123999E-13</v>
+      </c>
+      <c r="F21" s="5">
+        <v>1590.0187686751101</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="8"/>
+      <c r="B22" s="13">
+        <v>-4.1139883354204397E-6</v>
+      </c>
+      <c r="C22" s="14">
+        <v>9.0073473549481295E-7</v>
+      </c>
+      <c r="D22" s="14">
+        <v>-4.5673694743885296</v>
+      </c>
+      <c r="E22" s="14">
+        <v>5.5608248797898501E-6</v>
+      </c>
+      <c r="F22" s="8">
+        <v>19.185733504671902</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="3"/>
+      <c r="B23" s="11">
+        <v>-5.9417709224784699E-5</v>
+      </c>
+      <c r="C23" s="12">
+        <v>6.8262560725836901E-5</v>
+      </c>
+      <c r="D23" s="12">
+        <v>-0.87042895245937602</v>
+      </c>
+      <c r="E23" s="12">
+        <v>0.38421818382580097</v>
+      </c>
+      <c r="F23" s="3">
+        <v>2030.4170856123501</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="8"/>
+      <c r="B24" s="13">
+        <v>-2.7682109669568202E-4</v>
+      </c>
+      <c r="C24" s="14">
+        <v>3.9310684840902299E-4</v>
+      </c>
+      <c r="D24" s="14">
+        <v>-0.70418792706366895</v>
+      </c>
+      <c r="E24" s="14">
+        <v>0.48182155663255799</v>
+      </c>
+      <c r="F24" s="8">
+        <v>6995.1243416016996</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="3"/>
+      <c r="B25" s="11">
+        <v>-1.36217611298399E-4</v>
+      </c>
+      <c r="C25" s="12">
+        <v>3.8441639247682999E-5</v>
+      </c>
+      <c r="D25" s="12">
+        <v>-3.5434912236894101</v>
+      </c>
+      <c r="E25" s="12">
+        <v>4.0853752975595698E-4</v>
+      </c>
+      <c r="F25" s="3">
+        <v>891.31596090691005</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="10"/>
+      <c r="B26" s="15">
+        <v>-6.5529252914953303E-4</v>
+      </c>
+      <c r="C26" s="16">
+        <v>4.0631751038646101E-5</v>
+      </c>
+      <c r="D26" s="16">
+        <v>-16.127597565910101</v>
+      </c>
+      <c r="E26" s="16">
+        <v>1.3437749374070399E-56</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1640.3779969520101</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="23"/>
     </row>
     <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D29" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="20" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1099,87 +1339,147 @@
       <c r="A30" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="5"/>
+      <c r="B30" s="17">
+        <v>-1.14427743922528E-3</v>
+      </c>
+      <c r="C30" s="18">
+        <v>2.0292434099824101E-4</v>
+      </c>
+      <c r="D30" s="18">
+        <v>-5.6389363326068498</v>
+      </c>
+      <c r="E30" s="18">
+        <v>1.7292384641139798E-8</v>
+      </c>
+      <c r="F30" s="5">
+        <v>5199.3734372341196</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="8"/>
+      <c r="B31" s="13">
+        <v>-1.9626760055494198E-6</v>
+      </c>
+      <c r="C31" s="14">
+        <v>6.0382317891470204E-7</v>
+      </c>
+      <c r="D31" s="14">
+        <v>-3.2504151448393999</v>
+      </c>
+      <c r="E31" s="14">
+        <v>1.1744542435194599E-3</v>
+      </c>
+      <c r="F31" s="8">
+        <v>6.7681340896712401</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="3"/>
+      <c r="B32" s="11">
+        <v>5.1832020275035401E-4</v>
+      </c>
+      <c r="C32" s="12">
+        <v>2.47621548924408E-4</v>
+      </c>
+      <c r="D32" s="12">
+        <v>2.0931950591609598</v>
+      </c>
+      <c r="E32" s="12">
+        <v>3.6434677406707999E-2</v>
+      </c>
+      <c r="F32" s="3">
+        <v>6404.9141049283498</v>
+      </c>
     </row>
     <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="8"/>
+      <c r="B33" s="13">
+        <v>-6.9154691382022002E-3</v>
+      </c>
+      <c r="C33" s="14">
+        <v>2.7898036325691802E-3</v>
+      </c>
+      <c r="D33" s="14">
+        <v>-2.4788372405385402</v>
+      </c>
+      <c r="E33" s="14">
+        <v>1.3311337713832E-2</v>
+      </c>
+      <c r="F33" s="8">
+        <v>31269.4171423511</v>
+      </c>
     </row>
     <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="3"/>
+      <c r="B34" s="11">
+        <v>-2.2240427004653501E-3</v>
+      </c>
+      <c r="C34" s="12">
+        <v>2.5626949529253701E-4</v>
+      </c>
+      <c r="D34" s="12">
+        <v>-8.6785307706114505</v>
+      </c>
+      <c r="E34" s="12">
+        <v>6.3521953820121697E-18</v>
+      </c>
+      <c r="F34" s="3">
+        <v>4307.55355199734</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="10"/>
+      <c r="B35" s="15">
+        <v>-1.0833355130910301E-3</v>
+      </c>
+      <c r="C35" s="16">
+        <v>1.5508883867053E-4</v>
+      </c>
+      <c r="D35" s="16">
+        <v>-6.9852577553466801</v>
+      </c>
+      <c r="E35" s="16">
+        <v>2.9964209680288401E-12</v>
+      </c>
+      <c r="F35" s="10">
+        <v>4082.4329952732</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="23"/>
     </row>
     <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="23" t="s">
+      <c r="F38" s="20" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1187,87 +1487,147 @@
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="5"/>
+      <c r="B39" s="17">
+        <v>-7.20468473730332E-5</v>
+      </c>
+      <c r="C39" s="18">
+        <v>1.7544899985278298E-5</v>
+      </c>
+      <c r="D39" s="18">
+        <v>-4.1064267925999296</v>
+      </c>
+      <c r="E39" s="18">
+        <v>4.0308612249094597E-5</v>
+      </c>
+      <c r="F39" s="5">
+        <v>2718.4749115980799</v>
+      </c>
     </row>
     <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="8"/>
+      <c r="B40" s="13">
+        <v>-2.14244772480682E-7</v>
+      </c>
+      <c r="C40" s="14">
+        <v>1.46933612651502E-6</v>
+      </c>
+      <c r="D40" s="14">
+        <v>-0.145810593379222</v>
+      </c>
+      <c r="E40" s="14">
+        <v>0.88408280123921901</v>
+      </c>
+      <c r="F40" s="8">
+        <v>23.2575460112851</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="3"/>
+      <c r="B41" s="11">
+        <v>1.2286303289576699E-4</v>
+      </c>
+      <c r="C41" s="12">
+        <v>4.0738367764035102E-5</v>
+      </c>
+      <c r="D41" s="12">
+        <v>3.0159046530144402</v>
+      </c>
+      <c r="E41" s="12">
+        <v>2.5818839511783302E-3</v>
+      </c>
+      <c r="F41" s="3">
+        <v>3124.2339637472401</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B42" s="13"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="8"/>
+      <c r="B42" s="13">
+        <v>5.3350420833651999E-4</v>
+      </c>
+      <c r="C42" s="14">
+        <v>2.8501978410967001E-4</v>
+      </c>
+      <c r="D42" s="14">
+        <v>1.8718146531583899</v>
+      </c>
+      <c r="E42" s="14">
+        <v>6.1799933900303902E-2</v>
+      </c>
+      <c r="F42" s="8">
+        <v>21499.582305792199</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="3"/>
+      <c r="B43" s="11">
+        <v>-2.3555680776990901E-4</v>
+      </c>
+      <c r="C43" s="12">
+        <v>6.4463575791571197E-5</v>
+      </c>
+      <c r="D43" s="12">
+        <v>-3.6541070655393102</v>
+      </c>
+      <c r="E43" s="12">
+        <v>2.62779370745074E-4</v>
+      </c>
+      <c r="F43" s="3">
+        <v>4009.0969444971802</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="15"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="10"/>
+      <c r="B44" s="15">
+        <v>-2.6390989259174102E-4</v>
+      </c>
+      <c r="C44" s="16">
+        <v>1.82560577443761E-5</v>
+      </c>
+      <c r="D44" s="16">
+        <v>-14.456017629164201</v>
+      </c>
+      <c r="E44" s="16">
+        <v>6.67007772888855E-47</v>
+      </c>
+      <c r="F44" s="10">
+        <v>2597.0656846379902</v>
+      </c>
     </row>
     <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
+      <c r="A46" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="22"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="23"/>
     </row>
     <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="23" t="s">
+      <c r="C47" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D47" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="23" t="s">
+      <c r="E47" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="23" t="s">
+      <c r="F47" s="20" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1275,87 +1635,147 @@
       <c r="A48" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="5"/>
+      <c r="B48" s="17">
+        <v>-9.7045695885151998E-3</v>
+      </c>
+      <c r="C48" s="18">
+        <v>3.0239858482473099E-3</v>
+      </c>
+      <c r="D48" s="18">
+        <v>-3.2091980834301701</v>
+      </c>
+      <c r="E48" s="18">
+        <v>1.33613614970658E-3</v>
+      </c>
+      <c r="F48" s="5">
+        <v>83333.480376335705</v>
+      </c>
     </row>
     <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B49" s="13"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="8"/>
+      <c r="B49" s="13">
+        <v>-2.4334505105973898E-6</v>
+      </c>
+      <c r="C49" s="14">
+        <v>1.3312232534997101E-5</v>
+      </c>
+      <c r="D49" s="14">
+        <v>-0.182798077197043</v>
+      </c>
+      <c r="E49" s="14">
+        <v>0.85503145209519105</v>
+      </c>
+      <c r="F49" s="8">
+        <v>334.73251957622</v>
+      </c>
     </row>
     <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="3"/>
+      <c r="B50" s="11">
+        <v>-1.38129559332404E-2</v>
+      </c>
+      <c r="C50" s="12">
+        <v>1.8310185803623699E-3</v>
+      </c>
+      <c r="D50" s="12">
+        <v>-7.5438644268190602</v>
+      </c>
+      <c r="E50" s="12">
+        <v>1.34249770400575E-13</v>
+      </c>
+      <c r="F50" s="3">
+        <v>23225.446588369399</v>
+      </c>
     </row>
     <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="8"/>
+      <c r="B51" s="13">
+        <v>-4.8108862968992902E-2</v>
+      </c>
+      <c r="C51" s="14">
+        <v>9.5533344532245604E-3</v>
+      </c>
+      <c r="D51" s="14">
+        <v>-5.0358189807491298</v>
+      </c>
+      <c r="E51" s="14">
+        <v>5.5990890938968095E-7</v>
+      </c>
+      <c r="F51" s="8">
+        <v>355759.47212060599</v>
+      </c>
     </row>
     <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="3"/>
+      <c r="B52" s="11">
+        <v>-4.2018570963783999E-3</v>
+      </c>
+      <c r="C52" s="12">
+        <v>1.30870922518188E-2</v>
+      </c>
+      <c r="D52" s="12">
+        <v>-0.32106880699908302</v>
+      </c>
+      <c r="E52" s="12">
+        <v>0.74823662011776104</v>
+      </c>
+      <c r="F52" s="3">
+        <v>75545.960301028594</v>
+      </c>
     </row>
     <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="15"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
-      <c r="E53" s="16"/>
-      <c r="F53" s="10"/>
+      <c r="B53" s="15">
+        <v>-6.5455506667005904E-3</v>
+      </c>
+      <c r="C53" s="16">
+        <v>8.0514617547797901E-4</v>
+      </c>
+      <c r="D53" s="16">
+        <v>-8.1296426239804198</v>
+      </c>
+      <c r="E53" s="16">
+        <v>6.9074524738803303E-16</v>
+      </c>
+      <c r="F53" s="10">
+        <v>35012.221031269997</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="20" t="s">
+      <c r="A55" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-      <c r="F55" s="22"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="23"/>
     </row>
     <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="23" t="s">
+      <c r="C56" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D56" s="23" t="s">
+      <c r="D56" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="23" t="s">
+      <c r="E56" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F56" s="23" t="s">
+      <c r="F56" s="20" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1363,87 +1783,147 @@
       <c r="A57" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="17"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="5"/>
+      <c r="B57" s="17">
+        <v>1.12583395555123E-2</v>
+      </c>
+      <c r="C57" s="18">
+        <v>1.17060502585581E-3</v>
+      </c>
+      <c r="D57" s="18">
+        <v>9.6175390561658904</v>
+      </c>
+      <c r="E57" s="18">
+        <v>8.8071297878194E-22</v>
+      </c>
+      <c r="F57" s="5">
+        <v>45564.455101268803</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="8"/>
+      <c r="B58" s="13">
+        <v>-8.6452565927365698E-6</v>
+      </c>
+      <c r="C58" s="14">
+        <v>2.2962054341138799E-6</v>
+      </c>
+      <c r="D58" s="14">
+        <v>-3.7650187845987899</v>
+      </c>
+      <c r="E58" s="14">
+        <v>1.7992725513474899E-4</v>
+      </c>
+      <c r="F58" s="8">
+        <v>43.802598885109497</v>
+      </c>
     </row>
     <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B59" s="11"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="3"/>
+      <c r="B59" s="11">
+        <v>5.57437863369485E-2</v>
+      </c>
+      <c r="C59" s="12">
+        <v>5.0515579889821999E-3</v>
+      </c>
+      <c r="D59" s="12">
+        <v>11.0349691042901</v>
+      </c>
+      <c r="E59" s="12">
+        <v>2.7969983576552902E-26</v>
+      </c>
+      <c r="F59" s="3">
+        <v>99861.544541532101</v>
+      </c>
     </row>
     <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B60" s="13"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="8"/>
+      <c r="B60" s="13">
+        <v>-4.5402422345628003E-2</v>
+      </c>
+      <c r="C60" s="14">
+        <v>7.1487346660958498E-3</v>
+      </c>
+      <c r="D60" s="14">
+        <v>-6.3511130943154299</v>
+      </c>
+      <c r="E60" s="14">
+        <v>3.35851039422056E-10</v>
+      </c>
+      <c r="F60" s="8">
+        <v>180761.985891916</v>
+      </c>
     </row>
     <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B61" s="11"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="3"/>
+      <c r="B61" s="11">
+        <v>3.5810202025983E-2</v>
+      </c>
+      <c r="C61" s="12">
+        <v>1.83456667740827E-3</v>
+      </c>
+      <c r="D61" s="12">
+        <v>19.519705915825799</v>
+      </c>
+      <c r="E61" s="12">
+        <v>7.3283592949574701E-73</v>
+      </c>
+      <c r="F61" s="3">
+        <v>61635.912264945502</v>
+      </c>
     </row>
     <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B62" s="15"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="10"/>
+      <c r="B62" s="15">
+        <v>-7.5048381918523801E-4</v>
+      </c>
+      <c r="C62" s="16">
+        <v>3.75881350453486E-4</v>
+      </c>
+      <c r="D62" s="16">
+        <v>-1.99659764518726</v>
+      </c>
+      <c r="E62" s="16">
+        <v>4.59842262797839E-2</v>
+      </c>
+      <c r="F62" s="10">
+        <v>13490.3400782752</v>
+      </c>
     </row>
     <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B64" s="21"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
-      <c r="F64" s="22"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="23"/>
     </row>
     <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="23" t="s">
+      <c r="C65" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="23" t="s">
+      <c r="D65" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="23" t="s">
+      <c r="E65" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F65" s="23" t="s">
+      <c r="F65" s="20" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1451,87 +1931,147 @@
       <c r="A66" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="17"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="5"/>
+      <c r="B66" s="17">
+        <v>4.0555506351992003E-3</v>
+      </c>
+      <c r="C66" s="18">
+        <v>3.09446796985865E-4</v>
+      </c>
+      <c r="D66" s="18">
+        <v>13.1058090589461</v>
+      </c>
+      <c r="E66" s="18">
+        <v>4.7490391451837902E-39</v>
+      </c>
+      <c r="F66" s="5">
+        <v>16179.052775292301</v>
+      </c>
     </row>
     <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B67" s="13"/>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="8"/>
+      <c r="B67" s="13">
+        <v>-9.3059608406865204E-7</v>
+      </c>
+      <c r="C67" s="14">
+        <v>1.3579968146154201E-6</v>
+      </c>
+      <c r="D67" s="14">
+        <v>-0.68527118329963999</v>
+      </c>
+      <c r="E67" s="14">
+        <v>0.493323777404163</v>
+      </c>
+      <c r="F67" s="8">
+        <v>12.244388666777301</v>
+      </c>
     </row>
     <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B68" s="11"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="3"/>
+      <c r="B68" s="11">
+        <v>1.0581087795862599E-2</v>
+      </c>
+      <c r="C68" s="12">
+        <v>1.47620205550583E-3</v>
+      </c>
+      <c r="D68" s="12">
+        <v>7.1677774437435602</v>
+      </c>
+      <c r="E68" s="12">
+        <v>1.1217553601563001E-12</v>
+      </c>
+      <c r="F68" s="3">
+        <v>29106.4399186759</v>
+      </c>
     </row>
     <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B69" s="13"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="8"/>
+      <c r="B69" s="13">
+        <v>1.1321084057201201E-2</v>
+      </c>
+      <c r="C69" s="14">
+        <v>2.4038964090562099E-3</v>
+      </c>
+      <c r="D69" s="14">
+        <v>4.7094725107751101</v>
+      </c>
+      <c r="E69" s="14">
+        <v>2.6931852359086298E-6</v>
+      </c>
+      <c r="F69" s="8">
+        <v>80955.254324042602</v>
+      </c>
     </row>
     <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B70" s="11"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="3"/>
+      <c r="B70" s="11">
+        <v>5.7821156973912498E-3</v>
+      </c>
+      <c r="C70" s="12">
+        <v>4.7273918887139098E-4</v>
+      </c>
+      <c r="D70" s="12">
+        <v>12.231090278754699</v>
+      </c>
+      <c r="E70" s="12">
+        <v>2.2383109882270199E-33</v>
+      </c>
+      <c r="F70" s="3">
+        <v>13899.054092639701</v>
+      </c>
     </row>
     <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B71" s="15"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="10"/>
+      <c r="B71" s="15">
+        <v>3.9108555414290601E-5</v>
+      </c>
+      <c r="C71" s="16">
+        <v>1.1225868230551501E-4</v>
+      </c>
+      <c r="D71" s="16">
+        <v>0.348378892492749</v>
+      </c>
+      <c r="E71" s="16">
+        <v>0.72756763713101802</v>
+      </c>
+      <c r="F71" s="10">
+        <v>5552.6894241830196</v>
+      </c>
     </row>
     <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="20" t="s">
+      <c r="A73" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B73" s="21"/>
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="22"/>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="23"/>
     </row>
     <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C74" s="23" t="s">
+      <c r="C74" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D74" s="23" t="s">
+      <c r="D74" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E74" s="23" t="s">
+      <c r="E74" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F74" s="23" t="s">
+      <c r="F74" s="20" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1539,87 +2079,147 @@
       <c r="A75" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B75" s="17"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="5"/>
+      <c r="B75" s="17">
+        <v>-4.1522849311473398E-3</v>
+      </c>
+      <c r="C75" s="18">
+        <v>9.8709405155771694E-3</v>
+      </c>
+      <c r="D75" s="18">
+        <v>-0.42065747682246502</v>
+      </c>
+      <c r="E75" s="18">
+        <v>0.67402179621430802</v>
+      </c>
+      <c r="F75" s="5">
+        <v>38966.8380696401</v>
+      </c>
     </row>
     <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B76" s="13"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="8"/>
+      <c r="B76" s="13">
+        <v>-8.4700510660339196E-7</v>
+      </c>
+      <c r="C76" s="14">
+        <v>1.74473514090757E-6</v>
+      </c>
+      <c r="D76" s="14">
+        <v>-0.48546343037648598</v>
+      </c>
+      <c r="E76" s="14">
+        <v>0.62810112817269403</v>
+      </c>
+      <c r="F76" s="8">
+        <v>2.2958126697464398</v>
+      </c>
     </row>
     <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B77" s="11"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="3"/>
+      <c r="B77" s="11">
+        <v>-2.98612991835937E-2</v>
+      </c>
+      <c r="C77" s="12">
+        <v>1.0756311024142901E-2</v>
+      </c>
+      <c r="D77" s="12">
+        <v>-2.77616546384434</v>
+      </c>
+      <c r="E77" s="12">
+        <v>5.6247036009319396E-3</v>
+      </c>
+      <c r="F77" s="3">
+        <v>42624.404282155898</v>
+      </c>
     </row>
     <row r="78" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B78" s="13"/>
-      <c r="C78" s="14"/>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-      <c r="F78" s="8"/>
+      <c r="B78" s="13">
+        <v>-6.2093160730712797E-2</v>
+      </c>
+      <c r="C78" s="14">
+        <v>1.9020813287213001E-2</v>
+      </c>
+      <c r="D78" s="14">
+        <v>-3.2644850560862002</v>
+      </c>
+      <c r="E78" s="14">
+        <v>1.1804724566269399E-3</v>
+      </c>
+      <c r="F78" s="8">
+        <v>139542.73883348901</v>
+      </c>
     </row>
     <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B79" s="11"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="3"/>
+      <c r="B79" s="11">
+        <v>-1.3855229593255E-3</v>
+      </c>
+      <c r="C79" s="12">
+        <v>5.3144715812841999E-3</v>
+      </c>
+      <c r="D79" s="12">
+        <v>-0.26070756765448599</v>
+      </c>
+      <c r="E79" s="12">
+        <v>0.79440163017462095</v>
+      </c>
+      <c r="F79" s="3">
+        <v>14616.341635573801</v>
+      </c>
     </row>
     <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B80" s="15"/>
-      <c r="C80" s="16"/>
-      <c r="D80" s="16"/>
-      <c r="E80" s="16"/>
-      <c r="F80" s="10"/>
+      <c r="B80" s="15">
+        <v>-2.4478274403928999E-2</v>
+      </c>
+      <c r="C80" s="16">
+        <v>2.3039906122051299E-2</v>
+      </c>
+      <c r="D80" s="16">
+        <v>-1.0624294332736499</v>
+      </c>
+      <c r="E80" s="16">
+        <v>0.28816015205290402</v>
+      </c>
+      <c r="F80" s="10">
+        <v>39036.920081386597</v>
+      </c>
     </row>
     <row r="82" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="20" t="s">
+      <c r="A82" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B82" s="21"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="22"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="23"/>
     </row>
     <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C83" s="23" t="s">
+      <c r="C83" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="23" t="s">
+      <c r="D83" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E83" s="23" t="s">
+      <c r="E83" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F83" s="23" t="s">
+      <c r="F83" s="20" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1627,61 +2227,121 @@
       <c r="A84" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="17"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="18"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="5"/>
+      <c r="B84" s="17">
+        <v>-4.2794159866026997E-3</v>
+      </c>
+      <c r="C84" s="18">
+        <v>4.32787753939166E-4</v>
+      </c>
+      <c r="D84" s="18">
+        <v>-9.8880246671772092</v>
+      </c>
+      <c r="E84" s="18">
+        <v>4.9278681626700799E-23</v>
+      </c>
+      <c r="F84" s="5">
+        <v>22686.990603631701</v>
+      </c>
     </row>
     <row r="85" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B85" s="13"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="8"/>
+      <c r="B85" s="13">
+        <v>-7.35489203473804E-5</v>
+      </c>
+      <c r="C85" s="14">
+        <v>7.37140659456634E-6</v>
+      </c>
+      <c r="D85" s="14">
+        <v>-9.9775964605717604</v>
+      </c>
+      <c r="E85" s="14">
+        <v>3.2771349824750999E-23</v>
+      </c>
+      <c r="F85" s="8">
+        <v>212.284268767828</v>
+      </c>
     </row>
     <row r="86" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B86" s="11"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="3"/>
+      <c r="B86" s="11">
+        <v>-2.9579605978916701E-3</v>
+      </c>
+      <c r="C86" s="12">
+        <v>2.04726946175294E-4</v>
+      </c>
+      <c r="D86" s="12">
+        <v>-14.448320815370201</v>
+      </c>
+      <c r="E86" s="12">
+        <v>1.3022992605623599E-46</v>
+      </c>
+      <c r="F86" s="3">
+        <v>13331.221100916</v>
+      </c>
     </row>
     <row r="87" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B87" s="13"/>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14"/>
-      <c r="E87" s="14"/>
-      <c r="F87" s="8"/>
+      <c r="B87" s="13">
+        <v>-1.51094855368753E-2</v>
+      </c>
+      <c r="C87" s="14">
+        <v>1.42176497702383E-3</v>
+      </c>
+      <c r="D87" s="14">
+        <v>-10.6272736922412</v>
+      </c>
+      <c r="E87" s="14">
+        <v>4.6102990752876899E-26</v>
+      </c>
+      <c r="F87" s="8">
+        <v>78413.625214326297</v>
+      </c>
     </row>
     <row r="88" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B88" s="11"/>
-      <c r="C88" s="12"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="12"/>
-      <c r="F88" s="3"/>
+      <c r="B88" s="11">
+        <v>-1.1094282386017699E-2</v>
+      </c>
+      <c r="C88" s="12">
+        <v>8.4608598598917605E-4</v>
+      </c>
+      <c r="D88" s="12">
+        <v>-13.1124762373262</v>
+      </c>
+      <c r="E88" s="12">
+        <v>8.92651555714414E-39</v>
+      </c>
+      <c r="F88" s="3">
+        <v>27802.594812777999</v>
+      </c>
     </row>
     <row r="89" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B89" s="15"/>
-      <c r="C89" s="16"/>
-      <c r="D89" s="16"/>
-      <c r="E89" s="16"/>
-      <c r="F89" s="10"/>
+      <c r="B89" s="15">
+        <v>-2.8978168529865001E-3</v>
+      </c>
+      <c r="C89" s="16">
+        <v>1.5583351905433301E-4</v>
+      </c>
+      <c r="D89" s="16">
+        <v>-18.595594006807701</v>
+      </c>
+      <c r="E89" s="16">
+        <v>2.1362557601879899E-76</v>
+      </c>
+      <c r="F89" s="10">
+        <v>10663.183167069499</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1708,7 +2368,7 @@
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
@@ -1719,35 +2379,35 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1757,7 +2417,7 @@
       <c r="E3" s="18"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
@@ -1767,7 +2427,7 @@
       <c r="E4" s="14"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1777,7 +2437,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
@@ -1787,7 +2447,7 @@
       <c r="E6" s="14"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1797,7 +2457,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>5</v>
       </c>
@@ -1807,35 +2467,35 @@
       <c r="E8" s="16"/>
       <c r="F8" s="10"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>0</v>
       </c>
@@ -1845,7 +2505,7 @@
       <c r="E12" s="18"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>1</v>
       </c>
@@ -1855,7 +2515,7 @@
       <c r="E13" s="14"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>2</v>
       </c>
@@ -1865,7 +2525,7 @@
       <c r="E14" s="12"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>3</v>
       </c>
@@ -1875,7 +2535,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
@@ -1885,7 +2545,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>5</v>
       </c>
@@ -1895,35 +2555,35 @@
       <c r="E17" s="16"/>
       <c r="F17" s="10"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="23"/>
+    </row>
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>0</v>
       </c>
@@ -1933,7 +2593,7 @@
       <c r="E21" s="18"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>1</v>
       </c>
@@ -1943,7 +2603,7 @@
       <c r="E22" s="14"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>2</v>
       </c>
@@ -1953,7 +2613,7 @@
       <c r="E23" s="12"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>3</v>
       </c>
@@ -1963,7 +2623,7 @@
       <c r="E24" s="14"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>4</v>
       </c>
@@ -1973,7 +2633,7 @@
       <c r="E25" s="12"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>5</v>
       </c>
@@ -1983,35 +2643,35 @@
       <c r="E26" s="16"/>
       <c r="F26" s="10"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="22"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="23"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D29" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>0</v>
       </c>
@@ -2021,7 +2681,7 @@
       <c r="E30" s="18"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>1</v>
       </c>
@@ -2031,7 +2691,7 @@
       <c r="E31" s="14"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>2</v>
       </c>
@@ -2041,7 +2701,7 @@
       <c r="E32" s="12"/>
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>3</v>
       </c>
@@ -2051,7 +2711,7 @@
       <c r="E33" s="14"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>4</v>
       </c>
@@ -2061,7 +2721,7 @@
       <c r="E34" s="12"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>5</v>
       </c>
@@ -2071,35 +2731,35 @@
       <c r="E35" s="16"/>
       <c r="F35" s="10"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="22"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="23"/>
+    </row>
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F38" s="23" t="s">
+      <c r="F38" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
@@ -2109,7 +2769,7 @@
       <c r="E39" s="18"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>1</v>
       </c>
@@ -2119,7 +2779,7 @@
       <c r="E40" s="14"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>2</v>
       </c>
@@ -2129,7 +2789,7 @@
       <c r="E41" s="12"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>3</v>
       </c>
@@ -2139,7 +2799,7 @@
       <c r="E42" s="14"/>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>4</v>
       </c>
@@ -2149,7 +2809,7 @@
       <c r="E43" s="12"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>5</v>
       </c>
@@ -2159,35 +2819,35 @@
       <c r="E44" s="16"/>
       <c r="F44" s="10"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="22"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
+      <c r="F46" s="23"/>
+    </row>
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="23" t="s">
+      <c r="C47" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D47" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="23" t="s">
+      <c r="E47" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="23" t="s">
+      <c r="F47" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>0</v>
       </c>
@@ -2197,7 +2857,7 @@
       <c r="E48" s="18"/>
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>1</v>
       </c>
@@ -2207,7 +2867,7 @@
       <c r="E49" s="14"/>
       <c r="F49" s="8"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>2</v>
       </c>
@@ -2217,7 +2877,7 @@
       <c r="E50" s="12"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>3</v>
       </c>
@@ -2227,7 +2887,7 @@
       <c r="E51" s="14"/>
       <c r="F51" s="8"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>4</v>
       </c>
@@ -2237,7 +2897,7 @@
       <c r="E52" s="12"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>5</v>
       </c>
@@ -2247,35 +2907,35 @@
       <c r="E53" s="16"/>
       <c r="F53" s="10"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="20" t="s">
+    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-      <c r="F55" s="22"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="23"/>
+    </row>
+    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="23" t="s">
+      <c r="C56" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D56" s="23" t="s">
+      <c r="D56" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="23" t="s">
+      <c r="E56" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F56" s="23" t="s">
+      <c r="F56" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>0</v>
       </c>
@@ -2285,7 +2945,7 @@
       <c r="E57" s="18"/>
       <c r="F57" s="5"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>1</v>
       </c>
@@ -2295,7 +2955,7 @@
       <c r="E58" s="14"/>
       <c r="F58" s="8"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>2</v>
       </c>
@@ -2305,7 +2965,7 @@
       <c r="E59" s="12"/>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>3</v>
       </c>
@@ -2315,7 +2975,7 @@
       <c r="E60" s="14"/>
       <c r="F60" s="8"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>4</v>
       </c>
@@ -2325,7 +2985,7 @@
       <c r="E61" s="12"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>5</v>
       </c>
@@ -2335,35 +2995,35 @@
       <c r="E62" s="16"/>
       <c r="F62" s="10"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
+    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B64" s="21"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
-      <c r="F64" s="22"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="23"/>
+    </row>
+    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C65" s="23" t="s">
+      <c r="C65" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="23" t="s">
+      <c r="D65" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="23" t="s">
+      <c r="E65" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F65" s="23" t="s">
+      <c r="F65" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>0</v>
       </c>
@@ -2373,7 +3033,7 @@
       <c r="E66" s="18"/>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>1</v>
       </c>
@@ -2383,7 +3043,7 @@
       <c r="E67" s="14"/>
       <c r="F67" s="8"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>2</v>
       </c>
@@ -2393,7 +3053,7 @@
       <c r="E68" s="12"/>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>3</v>
       </c>
@@ -2403,7 +3063,7 @@
       <c r="E69" s="14"/>
       <c r="F69" s="8"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>4</v>
       </c>
@@ -2413,7 +3073,7 @@
       <c r="E70" s="12"/>
       <c r="F70" s="3"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>5</v>
       </c>
@@ -2423,35 +3083,35 @@
       <c r="E71" s="16"/>
       <c r="F71" s="10"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="20" t="s">
+    <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B73" s="21"/>
-      <c r="C73" s="21"/>
-      <c r="D73" s="21"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="22"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="23"/>
+    </row>
+    <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C74" s="23" t="s">
+      <c r="C74" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D74" s="23" t="s">
+      <c r="D74" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E74" s="23" t="s">
+      <c r="E74" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F74" s="23" t="s">
+      <c r="F74" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>0</v>
       </c>
@@ -2461,7 +3121,7 @@
       <c r="E75" s="18"/>
       <c r="F75" s="5"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>1</v>
       </c>
@@ -2471,7 +3131,7 @@
       <c r="E76" s="14"/>
       <c r="F76" s="8"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>2</v>
       </c>
@@ -2481,7 +3141,7 @@
       <c r="E77" s="12"/>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>3</v>
       </c>
@@ -2491,7 +3151,7 @@
       <c r="E78" s="14"/>
       <c r="F78" s="8"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>4</v>
       </c>
@@ -2501,7 +3161,7 @@
       <c r="E79" s="12"/>
       <c r="F79" s="3"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>5</v>
       </c>
@@ -2511,35 +3171,35 @@
       <c r="E80" s="16"/>
       <c r="F80" s="10"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="20" t="s">
+    <row r="82" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B82" s="21"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="21"/>
-      <c r="E82" s="21"/>
-      <c r="F82" s="22"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
+      <c r="F82" s="23"/>
+    </row>
+    <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C83" s="23" t="s">
+      <c r="C83" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D83" s="23" t="s">
+      <c r="D83" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E83" s="23" t="s">
+      <c r="E83" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F83" s="23" t="s">
+      <c r="F83" s="20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>0</v>
       </c>
@@ -2549,7 +3209,7 @@
       <c r="E84" s="18"/>
       <c r="F84" s="5"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>1</v>
       </c>
@@ -2559,7 +3219,7 @@
       <c r="E85" s="14"/>
       <c r="F85" s="8"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>2</v>
       </c>
@@ -2569,7 +3229,7 @@
       <c r="E86" s="12"/>
       <c r="F86" s="3"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>3</v>
       </c>
@@ -2579,7 +3239,7 @@
       <c r="E87" s="14"/>
       <c r="F87" s="8"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>4</v>
       </c>
@@ -2589,7 +3249,7 @@
       <c r="E88" s="12"/>
       <c r="F88" s="3"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>5</v>
       </c>

</xml_diff>